<commit_message>
Updating Value for Fish on Dell Computer
</commit_message>
<xml_diff>
--- a/testing.xlsx
+++ b/testing.xlsx
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="11">
   <si>
     <t xml:space="preserve">3000 Steps, 1000000 Fish</t>
   </si>
@@ -266,7 +266,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -442,11 +442,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="1"/>
-        <c:axId val="58954492"/>
-        <c:axId val="92718497"/>
+        <c:axId val="59198267"/>
+        <c:axId val="47047235"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="58954492"/>
+        <c:axId val="59198267"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -512,7 +512,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="92718497"/>
+        <c:crossAx val="47047235"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -520,7 +520,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="92718497"/>
+        <c:axId val="47047235"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -593,7 +593,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="58954492"/>
+        <c:crossAx val="59198267"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -621,7 +621,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -885,11 +885,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="1"/>
-        <c:axId val="70114121"/>
-        <c:axId val="79971847"/>
+        <c:axId val="68888104"/>
+        <c:axId val="67888233"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="70114121"/>
+        <c:axId val="68888104"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -955,7 +955,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="79971847"/>
+        <c:crossAx val="67888233"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -963,7 +963,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="79971847"/>
+        <c:axId val="67888233"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="20"/>
@@ -1037,7 +1037,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="70114121"/>
+        <c:crossAx val="68888104"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="5"/>
@@ -1090,7 +1090,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1330,11 +1330,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="1"/>
-        <c:axId val="70936679"/>
-        <c:axId val="20642305"/>
+        <c:axId val="83323246"/>
+        <c:axId val="59540214"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="70936679"/>
+        <c:axId val="83323246"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1400,7 +1400,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="20642305"/>
+        <c:crossAx val="59540214"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1408,7 +1408,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="20642305"/>
+        <c:axId val="59540214"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="250"/>
@@ -1483,7 +1483,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="70936679"/>
+        <c:crossAx val="83323246"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1546,9 +1546,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>500040</xdr:colOff>
+      <xdr:colOff>499680</xdr:colOff>
       <xdr:row>42</xdr:row>
-      <xdr:rowOff>22680</xdr:rowOff>
+      <xdr:rowOff>22320</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -1557,7 +1557,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="0" y="4883040"/>
-        <a:ext cx="5958360" cy="3474000"/>
+        <a:ext cx="5958000" cy="3473640"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -1576,9 +1576,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>713160</xdr:colOff>
+      <xdr:colOff>712800</xdr:colOff>
       <xdr:row>34</xdr:row>
-      <xdr:rowOff>114120</xdr:rowOff>
+      <xdr:rowOff>113760</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -1586,8 +1586,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="7192800" y="4120560"/>
-        <a:ext cx="5781600" cy="2727720"/>
+        <a:off x="7193520" y="4120560"/>
+        <a:ext cx="5782320" cy="2727360"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -1606,9 +1606,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>18</xdr:col>
-      <xdr:colOff>191880</xdr:colOff>
+      <xdr:colOff>191520</xdr:colOff>
       <xdr:row>33</xdr:row>
-      <xdr:rowOff>110520</xdr:rowOff>
+      <xdr:rowOff>110160</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -1616,8 +1616,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="14046120" y="3916800"/>
-        <a:ext cx="5550120" cy="2727720"/>
+        <a:off x="14048640" y="3916800"/>
+        <a:ext cx="5553720" cy="2727360"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -1638,10 +1638,10 @@
   <dimension ref="A1:L19"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="N17" activeCellId="0" sqref="N17"/>
+      <selection pane="topLeft" activeCell="N11" activeCellId="0" sqref="N11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.50390625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.51171875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="12"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="11.66"/>
@@ -1947,19 +1947,10 @@
       <c r="G11" s="0" t="s">
         <v>7</v>
       </c>
-      <c r="H11" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="I11" s="0" t="s">
-        <v>4</v>
-      </c>
-      <c r="J11" s="0" t="s">
-        <v>5</v>
-      </c>
-      <c r="K11" s="0" t="s">
+      <c r="H11" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="L11" s="0" t="s">
+      <c r="I11" s="1" t="s">
         <v>9</v>
       </c>
     </row>
@@ -1967,21 +1958,11 @@
       <c r="G12" s="1" t="n">
         <v>100</v>
       </c>
-      <c r="H12" s="2" t="n">
-        <v>0.622065</v>
-      </c>
-      <c r="I12" s="0" t="n">
-        <v>0.622087</v>
-      </c>
-      <c r="J12" s="0" t="n">
-        <v>0.622619</v>
-      </c>
-      <c r="K12" s="0" t="n">
-        <f aca="false">AVERAGE(H12:J12)</f>
-        <v>0.622257</v>
-      </c>
-      <c r="L12" s="2" t="n">
-        <v>0.049434</v>
+      <c r="H12" s="1" t="n">
+        <v>1.4437</v>
+      </c>
+      <c r="I12" s="2" t="n">
+        <v>0.0494</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1991,21 +1972,11 @@
       <c r="G13" s="0" t="n">
         <v>1000</v>
       </c>
-      <c r="H13" s="2" t="n">
-        <v>0.785081</v>
-      </c>
-      <c r="I13" s="2" t="n">
-        <v>0.786097</v>
-      </c>
-      <c r="J13" s="2" t="n">
-        <v>0.78248</v>
-      </c>
-      <c r="K13" s="0" t="n">
-        <f aca="false">AVERAGE(H13:J13)</f>
-        <v>0.784552666666667</v>
-      </c>
-      <c r="L13" s="0" t="n">
-        <v>0.247215</v>
+      <c r="H13" s="1" t="n">
+        <v>3.6846</v>
+      </c>
+      <c r="I13" s="1" t="n">
+        <v>0.2472</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2016,19 +1987,9 @@
         <v>10000</v>
       </c>
       <c r="H14" s="1" t="n">
-        <v>2.359709</v>
-      </c>
-      <c r="I14" s="2" t="n">
-        <v>2.36375</v>
-      </c>
-      <c r="J14" s="2" t="n">
-        <v>2.399141</v>
-      </c>
-      <c r="K14" s="0" t="n">
-        <f aca="false">AVERAGE(H14:J14)</f>
-        <v>2.3742</v>
-      </c>
-      <c r="L14" s="0" t="n">
+        <v>23.541971</v>
+      </c>
+      <c r="I14" s="1" t="n">
         <v>1.8972</v>
       </c>
     </row>
@@ -2039,21 +2000,11 @@
       <c r="G15" s="1" t="n">
         <v>100000</v>
       </c>
-      <c r="H15" s="2" t="n">
-        <v>18.048874</v>
+      <c r="H15" s="1" t="n">
+        <v>209.4251</v>
       </c>
       <c r="I15" s="2" t="n">
-        <v>18.050807</v>
-      </c>
-      <c r="J15" s="2" t="n">
-        <v>16.511226</v>
-      </c>
-      <c r="K15" s="0" t="n">
-        <f aca="false">AVERAGE(H15:J15)</f>
-        <v>17.536969</v>
-      </c>
-      <c r="L15" s="2" t="n">
-        <v>18.458616</v>
+        <v>18.4586</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2063,20 +2014,10 @@
       <c r="G16" s="1" t="n">
         <v>1000000</v>
       </c>
-      <c r="H16" s="2" t="n">
-        <v>170.900622</v>
+      <c r="H16" s="1" t="n">
+        <v>1574.5107</v>
       </c>
       <c r="I16" s="2" t="n">
-        <v>161.246245</v>
-      </c>
-      <c r="J16" s="2" t="n">
-        <v>164.981733</v>
-      </c>
-      <c r="K16" s="0" t="n">
-        <f aca="false">AVERAGE(H16:J16)</f>
-        <v>165.709533333333</v>
-      </c>
-      <c r="L16" s="2" t="n">
         <v>181.5163</v>
       </c>
     </row>
@@ -2088,21 +2029,12 @@
         <v>1500000</v>
       </c>
       <c r="H17" s="2" t="n">
-        <v>245.136412</v>
+        <v>1964.2471</v>
       </c>
       <c r="I17" s="2" t="n">
-        <v>233.863834</v>
-      </c>
-      <c r="J17" s="2" t="n">
-        <v>233.757665</v>
-      </c>
-      <c r="K17" s="0" t="n">
-        <f aca="false">AVERAGE(H17:J17)</f>
-        <v>237.585970333333</v>
-      </c>
-      <c r="L17" s="2" t="n">
-        <v>273.522789</v>
-      </c>
+        <v>273.5627</v>
+      </c>
+      <c r="J17" s="2"/>
     </row>
     <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B18" s="2"/>

</xml_diff>

<commit_message>
add tests for scheduling methods
</commit_message>
<xml_diff>
--- a/testing.xlsx
+++ b/testing.xlsx
@@ -1,20 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10910"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Desktop\High Performance Computing\CITS3402-Fish-School-Behaviour-Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aloysiusloh/Documents/GitHub/CITS3402-Fish-School-Behaviour-Project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C79137E9-3867-4529-814C-2F5B189EFC63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93E1800B-AE2D-4948-AF17-AEF344191FA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="660" windowWidth="25600" windowHeight="14280" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlchart.v2.0" hidden="1">Sheet1!$T$3:$T$6</definedName>
+    <definedName name="_xlchart.v2.1" hidden="1">Sheet1!$X$2</definedName>
+    <definedName name="_xlchart.v2.2" hidden="1">Sheet1!$X$3:$X$6</definedName>
+  </definedNames>
   <calcPr calcId="191029" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -36,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="17">
   <si>
     <t>3000 Steps, 1000000 Fish</t>
   </si>
@@ -70,12 +75,30 @@
   <si>
     <t>3000 Steps, 16 Threads, Dell Laptop</t>
   </si>
+  <si>
+    <t>3000 Steps, 16 Threads, 1000000 fish</t>
+  </si>
+  <si>
+    <t>Schedule</t>
+  </si>
+  <si>
+    <t>static</t>
+  </si>
+  <si>
+    <t>dynamic</t>
+  </si>
+  <si>
+    <t>guided</t>
+  </si>
+  <si>
+    <t>dynamic (chunk size = fish/threads)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -89,6 +112,12 @@
       <name val="Menlo"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Menlo"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -111,9 +140,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -202,7 +232,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="en-GB"/>
   <c:roundedCorners val="0"/>
   <c:style val="2"/>
   <c:chart>
@@ -607,7 +637,7 @@
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="en-GB"/>
   <c:roundedCorners val="0"/>
   <c:style val="2"/>
   <c:chart>
@@ -1121,7 +1151,7 @@
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="en-GB"/>
   <c:roundedCorners val="0"/>
   <c:style val="2"/>
   <c:chart>
@@ -1595,7 +1625,7 @@
 <file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="en-GB"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -2159,7 +2189,420 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-GB"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-GB"/>
+              <a:t>Scheduling Methods</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$X$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>t avg</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$T$3:$T$6</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>static</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>guided</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>dynamic</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>dynamic (chunk size = fish/threads)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$X$3:$X$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>153.52926299999999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>174.96572566666666</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>196.52163066666665</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>163.19115433333332</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-E6B2-2440-904F-EBD9B09A1879}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="2059797519"/>
+        <c:axId val="2060356367"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="2059797519"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2060356367"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="2060356367"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="200"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>runtime</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-GB" baseline="0"/>
+                  <a:t> (s)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-GB"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2059797519"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -2362,6 +2805,509 @@
       <a:solidFill>
         <a:schemeClr val="phClr"/>
       </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
       <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -2856,6 +3802,42 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>717550</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>425450</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>158750</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="7" name="Chart 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7E57624C-8684-ABD1-0814-C8F31EC1C239}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -3161,29 +4143,33 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L19"/>
+  <dimension ref="A1:X19"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="P8" sqref="P8"/>
+    <sheetView tabSelected="1" topLeftCell="H1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="T26" sqref="T26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.5" defaultRowHeight="15.6"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.5" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="12" customWidth="1"/>
-    <col min="2" max="2" width="11.69921875" customWidth="1"/>
-    <col min="3" max="5" width="10.796875" customWidth="1"/>
-    <col min="8" max="10" width="12.796875" customWidth="1"/>
+    <col min="2" max="2" width="11.6640625" customWidth="1"/>
+    <col min="3" max="5" width="10.83203125" customWidth="1"/>
+    <col min="8" max="10" width="12.83203125" customWidth="1"/>
+    <col min="20" max="20" width="32.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="G1" t="s">
         <v>1</v>
       </c>
+      <c r="T1" t="s">
+        <v>11</v>
+      </c>
     </row>
-    <row r="2" spans="1:12">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -3217,8 +4203,23 @@
       <c r="L2" t="s">
         <v>9</v>
       </c>
+      <c r="T2" t="s">
+        <v>12</v>
+      </c>
+      <c r="U2" t="s">
+        <v>3</v>
+      </c>
+      <c r="V2" t="s">
+        <v>4</v>
+      </c>
+      <c r="W2" t="s">
+        <v>5</v>
+      </c>
+      <c r="X2" t="s">
+        <v>6</v>
+      </c>
     </row>
-    <row r="3" spans="1:12">
+    <row r="3" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1</v>
       </c>
@@ -3254,8 +4255,24 @@
       <c r="L3" s="1">
         <v>1.7915E-2</v>
       </c>
+      <c r="T3" t="s">
+        <v>13</v>
+      </c>
+      <c r="U3" s="2">
+        <v>154.51690300000001</v>
+      </c>
+      <c r="V3" s="2">
+        <v>152.52462399999999</v>
+      </c>
+      <c r="W3" s="2">
+        <v>153.54626200000001</v>
+      </c>
+      <c r="X3">
+        <f>AVERAGE(U3:W3)</f>
+        <v>153.52926299999999</v>
+      </c>
     </row>
-    <row r="4" spans="1:12">
+    <row r="4" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A4">
         <f t="shared" ref="A4:A9" si="2">A3*2</f>
         <v>2</v>
@@ -3292,8 +4309,24 @@
       <c r="L4">
         <v>0.16783699999999999</v>
       </c>
+      <c r="T4" t="s">
+        <v>15</v>
+      </c>
+      <c r="U4" s="2">
+        <v>173.836174</v>
+      </c>
+      <c r="V4" s="2">
+        <v>176.43526700000001</v>
+      </c>
+      <c r="W4" s="2">
+        <v>174.62573599999999</v>
+      </c>
+      <c r="X4">
+        <f>AVERAGE(U4:W4)</f>
+        <v>174.96572566666666</v>
+      </c>
     </row>
-    <row r="5" spans="1:12">
+    <row r="5" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A5">
         <f t="shared" si="2"/>
         <v>4</v>
@@ -3330,8 +4363,24 @@
       <c r="L5">
         <v>1.6738230000000001</v>
       </c>
+      <c r="T5" t="s">
+        <v>14</v>
+      </c>
+      <c r="U5" s="2">
+        <v>194.601699</v>
+      </c>
+      <c r="V5" s="2">
+        <v>198.31782999999999</v>
+      </c>
+      <c r="W5" s="2">
+        <v>196.645363</v>
+      </c>
+      <c r="X5">
+        <f>AVERAGE(U5:W5)</f>
+        <v>196.52163066666665</v>
+      </c>
     </row>
-    <row r="6" spans="1:12">
+    <row r="6" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A6">
         <f t="shared" si="2"/>
         <v>8</v>
@@ -3368,8 +4417,24 @@
       <c r="L6" s="1">
         <v>16.618423</v>
       </c>
+      <c r="T6" t="s">
+        <v>16</v>
+      </c>
+      <c r="U6" s="1">
+        <v>163.345485</v>
+      </c>
+      <c r="V6" s="1">
+        <v>161.24624499999999</v>
+      </c>
+      <c r="W6" s="1">
+        <v>164.98173299999999</v>
+      </c>
+      <c r="X6">
+        <f>AVERAGE(U6:W6)</f>
+        <v>163.19115433333332</v>
+      </c>
     </row>
-    <row r="7" spans="1:12">
+    <row r="7" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A7">
         <f t="shared" si="2"/>
         <v>16</v>
@@ -3407,7 +4472,7 @@
         <v>161.642707</v>
       </c>
     </row>
-    <row r="8" spans="1:12">
+    <row r="8" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A8">
         <f t="shared" si="2"/>
         <v>32</v>
@@ -3445,7 +4510,7 @@
         <v>248.963638</v>
       </c>
     </row>
-    <row r="9" spans="1:12">
+    <row r="9" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A9">
         <f t="shared" si="2"/>
         <v>64</v>
@@ -3464,12 +4529,12 @@
         <v>176.1499</v>
       </c>
     </row>
-    <row r="10" spans="1:12">
+    <row r="10" spans="1:24" x14ac:dyDescent="0.2">
       <c r="G10" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:12">
+    <row r="11" spans="1:24" x14ac:dyDescent="0.2">
       <c r="G11" t="s">
         <v>7</v>
       </c>
@@ -3480,7 +4545,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:12">
+    <row r="12" spans="1:24" x14ac:dyDescent="0.2">
       <c r="G12">
         <v>100</v>
       </c>
@@ -3491,7 +4556,7 @@
         <v>4.9399999999999999E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:12">
+    <row r="13" spans="1:24" x14ac:dyDescent="0.2">
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
@@ -3505,7 +4570,7 @@
         <v>0.2472</v>
       </c>
     </row>
-    <row r="14" spans="1:12">
+    <row r="14" spans="1:24" x14ac:dyDescent="0.2">
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
@@ -3519,7 +4584,7 @@
         <v>1.8972</v>
       </c>
     </row>
-    <row r="15" spans="1:12">
+    <row r="15" spans="1:24" x14ac:dyDescent="0.2">
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
@@ -3533,7 +4598,7 @@
         <v>18.458600000000001</v>
       </c>
     </row>
-    <row r="16" spans="1:12">
+    <row r="16" spans="1:24" x14ac:dyDescent="0.2">
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
@@ -3547,7 +4612,7 @@
         <v>181.5163</v>
       </c>
     </row>
-    <row r="17" spans="2:10">
+    <row r="17" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
@@ -3562,12 +4627,12 @@
       </c>
       <c r="J17" s="1"/>
     </row>
-    <row r="18" spans="2:10">
+    <row r="18" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
     </row>
-    <row r="19" spans="2:10">
+    <row r="19" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>

</xml_diff>